<commit_message>
Updated supporting data to version 4.63
</commit_message>
<xml_diff>
--- a/src/excel/AntigenSupportingData- Cholera-508.xlsx
+++ b/src/excel/AntigenSupportingData- Cholera-508.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\Play CDS XML\Version 4.59 - 508\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\Play CDS XML\Version 4.63 - 508 - DRAFT\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495544B1-F9B7-4F7E-9035-0258BAA72952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0773BF4F-BDA2-4540-BB27-F160F913E21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,12 +600,6 @@
     <t>≥6 yrs to &lt;65 yrs</t>
   </si>
   <si>
-    <t>≥2 yrs - 4 d to &lt;65 yrs</t>
-  </si>
-  <si>
-    <t>≥2 yrs - 4 d to &lt;5 yrs</t>
-  </si>
-  <si>
     <t>50 mL</t>
   </si>
   <si>
@@ -657,9 +651,6 @@
     <t>6 years</t>
   </si>
   <si>
-    <t>Duplciate CVX 174 entry for those between 2 years and 6 years of age.</t>
-  </si>
-  <si>
     <t>Created a duplicate CVX 174 for those between the ages of 2 years and 6 years where only 50 mL should be used.</t>
   </si>
   <si>
@@ -691,6 +682,15 @@
   </si>
   <si>
     <t>Publication Date: 11/08/2024</t>
+  </si>
+  <si>
+    <t>Duplicate CVX 174 entry for those between 2 years and 6 years of age.</t>
+  </si>
+  <si>
+    <t>≥2 yrs - 4 days to &lt;65 yrs</t>
+  </si>
+  <si>
+    <t>≥2 yrs - 4 days to &lt;5 yrs</t>
   </si>
 </sst>
 </file>
@@ -2533,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C18" s="126"/>
       <c r="D18" s="126"/>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C19" s="126"/>
       <c r="D19" s="126"/>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C20" s="126"/>
       <c r="D20" s="126"/>
@@ -2578,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C21" s="126"/>
       <c r="D21" s="126"/>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C22" s="126"/>
       <c r="D22" s="126"/>
@@ -2728,7 +2728,7 @@
         <v>163</v>
       </c>
       <c r="D29" s="144" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>126</v>
@@ -2750,16 +2750,16 @@
         <v>123</v>
       </c>
       <c r="C30" s="143" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D30" s="144" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="E30" s="147" t="s">
         <v>126</v>
       </c>
       <c r="F30" s="147" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G30" s="148" t="s">
         <v>9</v>
@@ -2840,7 +2840,7 @@
         <v>4.59</v>
       </c>
       <c r="C1" s="142" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D3" s="61" t="s">
         <v>10</v>
@@ -2880,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>4.37</v>
       </c>
       <c r="C5" s="142" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,16 +2922,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>138</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F7" s="62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -2942,16 +2942,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>146</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F8" s="62" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2962,16 +2962,16 @@
         <v>3</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>138</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F9" s="62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2982,16 +2982,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>176</v>
-      </c>
       <c r="F10" s="62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3002,16 +3002,16 @@
         <v>5</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>138</v>
       </c>
       <c r="E11" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="62" t="s">
         <v>182</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3022,16 +3022,16 @@
         <v>6</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3042,16 +3042,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>138</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F13" s="62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -3705,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="145" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I15" s="104" t="s">
         <v>139</v>
@@ -3740,10 +3740,10 @@
         <v>141</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D17" s="138" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E17" s="138" t="s">
         <v>139</v>
@@ -3805,13 +3805,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="145" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C21" s="145" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" s="145" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E21" s="109" t="s">
         <v>10</v>
@@ -3981,7 +3981,7 @@
         <v>123</v>
       </c>
       <c r="C27" s="146" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D27" s="115" t="s">
         <v>139</v>
@@ -4005,10 +4005,10 @@
         <v>123</v>
       </c>
       <c r="C28" s="146" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D28" s="146" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E28" s="150" t="s">
         <v>10</v>
@@ -4046,7 +4046,7 @@
         <v>123</v>
       </c>
       <c r="C30" s="146" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D30" s="115" t="s">
         <v>10</v>

</xml_diff>